<commit_message>
batch definition updates again
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/sample_inputs/multiple_session_batch.xlsx
+++ b/sample_inputs/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\sample_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AEF1BB-59B5-4EC6-A21F-5AB14A148B18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EF7EB4-A838-408E-BA06-3F3BBCF3D6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="945" windowWidth="28935" windowHeight="18780" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17850" yWindow="135" windowWidth="16395" windowHeight="18780" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Parameter</t>
   </si>
@@ -125,12 +125,6 @@
     <t>Allow Backsliding</t>
   </si>
   <si>
-    <t>__dump</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
@@ -159,12 +153,6 @@
     <t>CostCurves</t>
   </si>
   <si>
-    <t>Session Output Folder Name</t>
-  </si>
-  <si>
-    <t>Database Dump Folder Name</t>
-  </si>
-  <si>
     <t>Demanded Shares File</t>
   </si>
   <si>
@@ -202,6 +190,12 @@
   </si>
   <si>
     <t>multiple_session_batch</t>
+  </si>
+  <si>
+    <t>Context Name</t>
+  </si>
+  <si>
+    <t>Context Folder Name</t>
   </si>
 </sst>
 </file>
@@ -697,8 +691,8 @@
   <dimension ref="A1:AG36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -800,8 +794,13 @@
       <c r="Q3" s="14"/>
     </row>
     <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -817,11 +816,14 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
     </row>
-    <row r="5" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="14"/>
+    <row r="5" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -837,76 +839,56 @@
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
     </row>
-    <row r="6" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-    </row>
-    <row r="7" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
+    <row r="6" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -924,32 +906,39 @@
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
     </row>
-    <row r="9" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-    </row>
-    <row r="10" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
+    <row r="9" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -966,34 +955,27 @@
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
     </row>
-    <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
+    <row r="11" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="12" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -1003,10 +985,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1032,10 +1014,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1061,10 +1043,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1084,16 +1066,16 @@
     </row>
     <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1119,10 +1101,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1148,10 +1130,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1177,10 +1159,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1203,13 +1185,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1235,10 +1217,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1264,10 +1246,10 @@
         <v>25</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1293,10 +1275,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1433,7 +1415,7 @@
     </row>
     <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>13</v>
@@ -1471,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1491,7 +1473,7 @@
     </row>
     <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>13</v>
@@ -1589,10 +1571,10 @@
         <v>26</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1618,10 +1600,10 @@
         <v>26</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>

</xml_diff>

<commit_message>
fixed batch run bug due to new input rows inching towards market class tree that ends in reg class leaves top level of producer-consumer iteration attempt is now run_producer_consumer()     doesn't call consumer module yet
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/sample_inputs/multiple_session_batch.xlsx
+++ b/sample_inputs/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\sample_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EF7EB4-A838-408E-BA06-3F3BBCF3D6FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419F1C9C-D0D0-4574-B2B8-904F2D07E0FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17850" yWindow="135" windowWidth="16395" windowHeight="18780" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13305" yWindow="780" windowWidth="24600" windowHeight="15765" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>Parameter</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Flat</t>
   </si>
   <si>
-    <t>Num Tech Options per Vehicle</t>
-  </si>
-  <si>
     <t>CostClouds
 CostCurves</t>
   </si>
@@ -196,6 +193,12 @@
   </si>
   <si>
     <t>Context Folder Name</t>
+  </si>
+  <si>
+    <t>Num Tech Options per ICE Vehicle</t>
+  </si>
+  <si>
+    <t>Num Tech Options per BEV Vehicle</t>
   </si>
 </sst>
 </file>
@@ -688,16 +691,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG36"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="17" width="21.28515625" style="11" customWidth="1"/>
@@ -776,7 +779,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -795,7 +798,7 @@
     </row>
     <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -818,7 +821,7 @@
     </row>
     <row r="5" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
@@ -914,7 +917,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>34</v>
@@ -985,10 +988,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1014,10 +1017,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1043,10 +1046,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1066,16 +1069,16 @@
     </row>
     <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1101,10 +1104,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1130,10 +1133,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1159,10 +1162,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1185,13 +1188,13 @@
         <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1217,10 +1220,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1275,10 +1278,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1415,7 +1418,7 @@
     </row>
     <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>13</v>
@@ -1442,69 +1445,77 @@
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
     </row>
-    <row r="29" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="8">
+        <v>10</v>
+      </c>
+      <c r="D29" s="8">
+        <v>5</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+    </row>
+    <row r="30" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="10" t="b">
+      <c r="C30" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-    </row>
-    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+    </row>
+    <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C31" s="8">
         <v>0.75</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D31" s="8">
         <v>0.75</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-    </row>
-    <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
@@ -1521,32 +1532,31 @@
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
     </row>
-    <row r="32" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-    </row>
-    <row r="33" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
+    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+    </row>
+    <row r="33" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
@@ -1563,38 +1573,31 @@
       <c r="R33" s="14"/>
       <c r="S33" s="14"/>
     </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
+    <row r="34" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
     </row>
     <row r="35" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>26</v>
@@ -1621,11 +1624,19 @@
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+    <row r="36" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
@@ -1642,6 +1653,27 @@
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
     </row>
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates to align with UML regarding fuels data added GHG_standards_fuels.py to store policy grams CO2/unit fuel fuel_scenario_annual_data is now fuels_context updates to batch definition files for getting rid of fuel scenarios and adding ghg standards fuels
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/sample_inputs/multiple_session_batch.xlsx
+++ b/sample_inputs/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\sample_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419F1C9C-D0D0-4574-B2B8-904F2D07E0FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8590BD-32F6-4C63-BC92-77EB9949C9AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13305" yWindow="780" windowWidth="24600" windowHeight="15765" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="4155" windowWidth="30945" windowHeight="15915" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Vehicles File</t>
   </si>
   <si>
-    <t>Fuel Scenarios File</t>
-  </si>
-  <si>
     <t>Fuel Scenario Annual Data File</t>
   </si>
   <si>
@@ -168,12 +165,6 @@
     <t>sample_inputs/fuels.csv</t>
   </si>
   <si>
-    <t>sample_inputs/fuel_scenarios.csv</t>
-  </si>
-  <si>
-    <t>sample_inputs/fuel_scenario_annual_data.csv</t>
-  </si>
-  <si>
     <t>sample_inputs/cost_curves.csv</t>
   </si>
   <si>
@@ -199,6 +190,15 @@
   </si>
   <si>
     <t>Num Tech Options per BEV Vehicle</t>
+  </si>
+  <si>
+    <t>sample_inputs/fuels_context.csv</t>
+  </si>
+  <si>
+    <t>GHG Standards Fuels File</t>
+  </si>
+  <si>
+    <t>sample_inputs/ghg_standards-fuels.csv</t>
   </si>
 </sst>
 </file>
@@ -694,8 +694,8 @@
   <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:C29"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +779,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -798,7 +798,7 @@
     </row>
     <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="5" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
@@ -917,10 +917,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -988,10 +988,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1017,10 +1017,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1046,10 +1046,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1069,16 +1069,16 @@
     </row>
     <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1098,16 +1098,16 @@
     </row>
     <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1133,10 +1133,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1154,18 +1154,18 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1183,18 +1183,18 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1212,47 +1212,47 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+    </row>
+    <row r="21" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-    </row>
-    <row r="21" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C21" s="10" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1271,17 +1271,17 @@
       <c r="S21" s="10"/>
     </row>
     <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>23</v>
+      <c r="A22" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>49</v>
+      <c r="C22" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>13</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="30" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>11</v>
@@ -1485,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>13</v>
@@ -1597,16 +1597,16 @@
     </row>
     <row r="35" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1626,16 +1626,16 @@
     </row>
     <row r="36" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>

</xml_diff>

<commit_message>
Added iteration control to batch file added required zev share input to batch file fixed a few minor issues got rid of non-pythonic code in run_omega_batch.py
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/sample_inputs/multiple_session_batch.xlsx
+++ b/sample_inputs/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\sample_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8590BD-32F6-4C63-BC92-77EB9949C9AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7930B9E3-A0EC-4C70-BD48-2382FDB6B32E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="4155" windowWidth="30945" windowHeight="15915" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="3300" windowWidth="14160" windowHeight="16785" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>Parameter</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>sample_inputs/ghg_standards-fuels.csv</t>
+  </si>
+  <si>
+    <t>ZEV Requirement File</t>
+  </si>
+  <si>
+    <t>sample_inputs/required_zev_share.csv</t>
+  </si>
+  <si>
+    <t>Iterate Producer-Consumer</t>
   </si>
 </sst>
 </file>
@@ -691,11 +700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG37"/>
+  <dimension ref="A1:AG39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
+      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,65 +1308,77 @@
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
     </row>
-    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+    </row>
+    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-    </row>
-    <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="8" t="b">
+      <c r="C24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+    </row>
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D24" s="8" t="b">
+      <c r="D25" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-    </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -1374,32 +1395,27 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-    </row>
-    <row r="27" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+    </row>
+    <row r="27" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1416,44 +1432,37 @@
       <c r="R27" s="14"/>
       <c r="S27" s="14"/>
     </row>
-    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="8">
-        <v>10</v>
-      </c>
-      <c r="D28" s="8">
-        <v>5</v>
-      </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
+    <row r="28" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="8">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D29" s="8">
         <v>5</v>
@@ -1474,69 +1483,77 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8">
+        <v>2</v>
+      </c>
+      <c r="D30" s="8">
+        <v>5</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+    </row>
+    <row r="31" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="10" t="b">
+      <c r="C31" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-    </row>
-    <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+    </row>
+    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C32" s="8">
         <v>0.75</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D32" s="8">
         <v>0.75</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-    </row>
-    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
@@ -1553,111 +1570,111 @@
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
     </row>
-    <row r="33" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-    </row>
-    <row r="34" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+    </row>
+    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+    </row>
+    <row r="35" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+    </row>
+    <row r="36" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
-    </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+    </row>
+    <row r="37" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C37" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-    </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-    </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -1674,6 +1691,56 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
+    <row r="38" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+    </row>
+    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>